<commit_message>
changes in scrum sheet
</commit_message>
<xml_diff>
--- a/Scrum Sheet.xlsx
+++ b/Scrum Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S8 CSA\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main_Project\Student-Performance-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61F77CF6-07D6-458A-9C50-C853E3DA50BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C027D7C8-D996-4F5C-9BB1-3C5D6B4DA46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1295,7 +1295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1511,11 +1511,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1672,6 +1687,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1719,20 +1740,29 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3954,17 +3984,17 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="66"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -3984,15 +4014,15 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="69"/>
+      <c r="A3" s="69"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -4012,15 +4042,15 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="70"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="74"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -4281,7 +4311,7 @@
       <c r="G12" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="91">
+      <c r="H12" s="65">
         <v>1</v>
       </c>
       <c r="I12" s="1"/>
@@ -4321,7 +4351,7 @@
       <c r="G13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H13" s="91">
+      <c r="H13" s="65">
         <v>1</v>
       </c>
       <c r="I13" s="1"/>
@@ -4361,7 +4391,7 @@
       <c r="G14" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="91">
+      <c r="H14" s="65">
         <v>2</v>
       </c>
       <c r="I14" s="1"/>
@@ -4401,7 +4431,7 @@
       <c r="G15" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="91">
+      <c r="H15" s="65">
         <v>2</v>
       </c>
       <c r="I15" s="1"/>
@@ -4441,7 +4471,7 @@
       <c r="G16" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="H16" s="91">
+      <c r="H16" s="65">
         <v>2</v>
       </c>
       <c r="I16" s="1"/>
@@ -4481,7 +4511,7 @@
       <c r="G17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H17" s="91">
+      <c r="H17" s="65">
         <v>3</v>
       </c>
       <c r="I17" s="1"/>
@@ -4521,7 +4551,7 @@
       <c r="G18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="91">
+      <c r="H18" s="65">
         <v>4</v>
       </c>
       <c r="I18" s="1"/>
@@ -4561,7 +4591,7 @@
       <c r="G19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="91">
+      <c r="H19" s="65">
         <v>5</v>
       </c>
       <c r="I19" s="1"/>
@@ -32255,28 +32285,28 @@
       <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="43.5" customHeight="1">
-      <c r="A2" s="78" t="str">
+      <c r="A2" s="80" t="str">
         <f>CONCATENATE("Sprint #",D5,"Tracking Sheet")</f>
         <v>Sprint #1Tracking Sheet</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="82"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1">
       <c r="A3" s="14"/>
@@ -32304,16 +32334,16 @@
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
       <c r="L4" s="19"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -32329,20 +32359,20 @@
       <c r="C5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="84">
         <v>1</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="85">
+      <c r="G5" s="76"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="87">
         <v>44974</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="77"/>
       <c r="L5" s="24"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
@@ -32357,16 +32387,16 @@
       <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="84"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="86"/>
       <c r="L6" s="24"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
@@ -32420,22 +32450,22 @@
       <c r="B9" s="14"/>
       <c r="C9" s="27"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="77"/>
       <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1">
@@ -32443,24 +32473,24 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="73" t="s">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="77"/>
       <c r="S10" s="28"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" customHeight="1">
@@ -32771,7 +32801,7 @@
       <c r="C19" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="76">
+      <c r="D19" s="78">
         <f>SUM(D14:D17)</f>
         <v>9</v>
       </c>
@@ -32839,7 +32869,7 @@
       <c r="C20" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D20" s="77"/>
+      <c r="D20" s="79"/>
       <c r="E20" s="45">
         <f t="shared" ref="E20:R20" si="5">FORECAST(E11,$R$25:$R$26,$O$25:$O$26)</f>
         <v>8.1</v>
@@ -34112,28 +34142,28 @@
       <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="43.5" customHeight="1">
-      <c r="A2" s="78" t="str">
+      <c r="A2" s="80" t="str">
         <f>CONCATENATE("Sprint #",D5,"Tracking Sheet")</f>
         <v>Sprint #2Tracking Sheet</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="82"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1">
       <c r="A3" s="14"/>
@@ -34161,16 +34191,16 @@
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
-      <c r="K4" s="74"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
       <c r="L4" s="19"/>
       <c r="M4" s="20"/>
       <c r="N4" s="20"/>
@@ -34186,20 +34216,20 @@
       <c r="C5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="84">
         <v>2</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="87">
+      <c r="G5" s="76"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="89">
         <v>44988</v>
       </c>
-      <c r="J5" s="74"/>
-      <c r="K5" s="75"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="77"/>
       <c r="L5" s="24"/>
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
@@ -34214,16 +34244,16 @@
       <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
-      <c r="K6" s="84"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="86"/>
       <c r="L6" s="24"/>
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
@@ -34277,22 +34307,22 @@
       <c r="B9" s="14"/>
       <c r="C9" s="27"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="77"/>
       <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1">
@@ -34300,24 +34330,24 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="73" t="s">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="77"/>
       <c r="S10" s="28"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" customHeight="1">
@@ -34583,7 +34613,7 @@
       <c r="C18" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="86">
+      <c r="D18" s="88">
         <f>SUM(D14:D17)</f>
         <v>7</v>
       </c>
@@ -34651,7 +34681,7 @@
       <c r="C19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="45">
         <f t="shared" ref="E19:R19" si="6">FORECAST(E11,$R$24:$R$25,$P$24:$P$25)</f>
         <v>6.3</v>
@@ -35883,8 +35913,8 @@
   </sheetPr>
   <dimension ref="A1:S988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:S2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -35926,28 +35956,28 @@
       <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="43.5" customHeight="1">
-      <c r="A2" s="92" t="str">
+      <c r="A2" s="91" t="str">
         <f>CONCATENATE("Sprint #",D5,"Tracking Sheet")</f>
         <v>Sprint #3Tracking Sheet</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="94"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="93"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1">
       <c r="A3" s="14"/>
@@ -35975,15 +36005,15 @@
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
@@ -36000,19 +36030,19 @@
       <c r="C5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="84">
         <v>3</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="89">
+      <c r="G5" s="76"/>
+      <c r="H5" s="94">
         <v>45002</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="75"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="77"/>
       <c r="K5" s="24"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
@@ -36028,15 +36058,15 @@
       <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="84" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="84"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="86"/>
       <c r="K6" s="24"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
@@ -36091,22 +36121,22 @@
       <c r="B9" s="14"/>
       <c r="C9" s="27"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="77"/>
       <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1">
@@ -36114,24 +36144,24 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="88" t="s">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="77"/>
+      <c r="L10" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="77"/>
       <c r="S10" s="28"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" customHeight="1">
@@ -36190,7 +36220,7 @@
       <c r="B12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="97" t="s">
         <v>43</v>
       </c>
       <c r="D12" s="23" t="s">
@@ -36257,13 +36287,13 @@
       <c r="A13" s="34">
         <v>1</v>
       </c>
-      <c r="B13" s="34">
+      <c r="B13" s="64">
         <v>6</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="96">
         <v>4</v>
       </c>
       <c r="E13" s="34"/>
@@ -36286,13 +36316,13 @@
       <c r="A14" s="34">
         <v>2</v>
       </c>
-      <c r="B14" s="34">
+      <c r="B14" s="64">
         <v>6</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="96">
         <v>4</v>
       </c>
       <c r="E14" s="34"/>
@@ -36315,13 +36345,13 @@
       <c r="A15" s="34">
         <v>3</v>
       </c>
-      <c r="B15" s="34">
+      <c r="B15" s="64">
         <v>6</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="34">
+      <c r="D15" s="96">
         <v>5</v>
       </c>
       <c r="E15" s="34"/>
@@ -36344,13 +36374,13 @@
       <c r="A16" s="34">
         <v>4</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="64">
         <v>6</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="96">
         <v>5</v>
       </c>
       <c r="E16" s="34"/>
@@ -36372,7 +36402,7 @@
     <row r="17" spans="1:19" ht="12.75" customHeight="1">
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
-      <c r="C17" s="37"/>
+      <c r="C17" s="98"/>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
       <c r="F17" s="34"/>
@@ -36396,7 +36426,7 @@
       <c r="C18" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="76">
+      <c r="D18" s="78">
         <f>SUM(D14:D17)</f>
         <v>14</v>
       </c>
@@ -36464,7 +36494,7 @@
       <c r="C19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="45">
         <f t="shared" ref="E19:R19" si="8">FORECAST(E11,$R$24:$R$25,$P$24:$P$25)</f>
         <v>12.6</v>
@@ -37737,27 +37767,27 @@
       <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="43.5" customHeight="1">
-      <c r="A2" s="78" t="str">
+      <c r="A2" s="80" t="str">
         <f>CONCATENATE("Sprint #",D5,"Tracking Sheet")</f>
         <v>Sprint #4Tracking Sheet</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="82"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1">
       <c r="A3" s="14"/>
@@ -37785,15 +37815,15 @@
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="74"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="19"/>
       <c r="L4" s="20"/>
       <c r="M4" s="20"/>
@@ -37810,19 +37840,19 @@
       <c r="C5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="84">
         <v>4</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="87">
+      <c r="G5" s="76"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="89">
         <v>45016</v>
       </c>
-      <c r="J5" s="75"/>
+      <c r="J5" s="77"/>
       <c r="K5" s="24"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
@@ -37838,15 +37868,15 @@
       <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="84"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="86"/>
       <c r="K6" s="24"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
@@ -37901,22 +37931,22 @@
       <c r="B9" s="14"/>
       <c r="C9" s="27"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="77"/>
       <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1">
@@ -37924,24 +37954,24 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="88" t="s">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="77"/>
       <c r="S10" s="28"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" customHeight="1">
@@ -38178,7 +38208,7 @@
       <c r="C17" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="76">
+      <c r="D17" s="78">
         <f>SUM(D14:D16)</f>
         <v>12</v>
       </c>
@@ -38246,7 +38276,7 @@
       <c r="C18" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="77"/>
+      <c r="D18" s="79"/>
       <c r="E18" s="45">
         <f t="shared" ref="E18:R18" si="6">FORECAST(E11,$R$23:$R$24,$O$23:$O$24)</f>
         <v>10.8</v>
@@ -39478,7 +39508,7 @@
   </sheetPr>
   <dimension ref="A1:S988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -39519,28 +39549,28 @@
       <c r="R1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="43.5" customHeight="1">
-      <c r="A2" s="78" t="str">
+      <c r="A2" s="80" t="str">
         <f>CONCATENATE("Sprint #",D5,"Tracking Sheet")</f>
         <v>Sprint #5Tracking Sheet</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="81"/>
+      <c r="O2" s="81"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="81"/>
+      <c r="R2" s="81"/>
+      <c r="S2" s="82"/>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1">
       <c r="A3" s="14"/>
@@ -39568,14 +39598,14 @@
       <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
       <c r="J4" s="19"/>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
@@ -39593,15 +39623,15 @@
       <c r="C5" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="84">
         <v>5</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="83" t="s">
+      <c r="E5" s="77"/>
+      <c r="F5" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="84"/>
+      <c r="G5" s="76"/>
+      <c r="H5" s="86"/>
       <c r="I5" s="51">
         <v>45030</v>
       </c>
@@ -39621,14 +39651,14 @@
       <c r="C6" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-      <c r="I6" s="84"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="86"/>
       <c r="J6" s="24"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
@@ -39684,22 +39714,22 @@
       <c r="B9" s="14"/>
       <c r="C9" s="27"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="73" t="s">
+      <c r="E9" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="75"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+      <c r="O9" s="76"/>
+      <c r="P9" s="76"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="77"/>
       <c r="S9" s="28"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1">
@@ -39707,24 +39737,24 @@
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="75"/>
-      <c r="J10" s="73" t="s">
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="75"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="76"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="77"/>
       <c r="S10" s="28"/>
     </row>
     <row r="11" spans="1:19" ht="12.75" customHeight="1">
@@ -39982,7 +40012,7 @@
       <c r="C18" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="76">
+      <c r="D18" s="78">
         <f>SUM(D14:D17)</f>
         <v>9</v>
       </c>
@@ -40050,7 +40080,7 @@
       <c r="C19" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="77"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="45">
         <f t="shared" ref="E19:R19" si="4">FORECAST(E11,$R$24:$R$25,$N$24:$N$25)</f>
         <v>8.1</v>
@@ -41300,10 +41330,10 @@
       <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" ht="39.75" customHeight="1">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="80"/>
+      <c r="B2" s="82"/>
       <c r="C2" s="54"/>
       <c r="D2" s="54"/>
       <c r="E2" s="54"/>

</xml_diff>

<commit_message>
Updated sprint 3 in scrum sheet
</commit_message>
<xml_diff>
--- a/Scrum Sheet.xlsx
+++ b/Scrum Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Main_Project\Student-Performance-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C027D7C8-D996-4F5C-9BB1-3C5D6B4DA46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF8A3D-3E50-4532-9C39-FE7BFBC2A98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sprint 3'!$A$12:$D$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Sprint 4'!$A$12:$D$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Sprint 5'!$A$12:$D$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Product Backlog'!$A$1:$I$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sprint 1 '!$A$1:$R$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Sprint 2'!$A$1:$S$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Sprint 3'!$A$1:$S$43</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Sprint 4'!$A$1:$S$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Sprint 5'!$A$1:$S$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -2556,34 +2562,34 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3942,8 +3948,8 @@
   </sheetPr>
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -32231,7 +32237,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="46" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -32242,14 +32248,14 @@
   </sheetPr>
   <dimension ref="A1:S989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A3" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="7.77734375" customWidth="1"/>
-    <col min="3" max="3" width="37.21875" customWidth="1"/>
+    <col min="3" max="3" width="59.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.21875" customWidth="1"/>
@@ -32613,7 +32619,7 @@
       </c>
       <c r="S12" s="33"/>
     </row>
-    <row r="13" spans="1:19" ht="25.5" customHeight="1">
+    <row r="13" spans="1:19" ht="25.2" customHeight="1">
       <c r="A13" s="34">
         <v>1</v>
       </c>
@@ -32650,7 +32656,7 @@
       <c r="R13" s="34"/>
       <c r="S13" s="35"/>
     </row>
-    <row r="14" spans="1:19" ht="25.5" customHeight="1">
+    <row r="14" spans="1:19" ht="25.2" customHeight="1">
       <c r="A14" s="34">
         <v>2</v>
       </c>
@@ -32722,7 +32728,7 @@
       <c r="R15" s="34"/>
       <c r="S15" s="35"/>
     </row>
-    <row r="16" spans="1:19" ht="25.5" customHeight="1">
+    <row r="16" spans="1:19" ht="25.2" customHeight="1">
       <c r="A16" s="34">
         <v>4</v>
       </c>
@@ -34086,9 +34092,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="51" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -34099,14 +34105,14 @@
   </sheetPr>
   <dimension ref="A1:S988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A10" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="7.77734375" customWidth="1"/>
-    <col min="3" max="3" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="53.88671875" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.21875" customWidth="1"/>
@@ -34491,13 +34497,19 @@
         <v>1</v>
       </c>
       <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
+      <c r="I13" s="34">
+        <v>1</v>
+      </c>
       <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
+      <c r="K13" s="34">
+        <v>1</v>
+      </c>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
+      <c r="O13" s="34">
+        <v>1</v>
+      </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
       <c r="R13" s="34"/>
@@ -34523,7 +34535,9 @@
         <v>1</v>
       </c>
       <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
+      <c r="H14" s="34">
+        <v>1</v>
+      </c>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
@@ -34555,14 +34569,22 @@
       <c r="H15" s="34"/>
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
+      <c r="K15" s="34">
+        <v>1</v>
+      </c>
+      <c r="L15" s="34">
+        <v>1</v>
+      </c>
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
       <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
+      <c r="P15" s="34">
+        <v>1</v>
+      </c>
       <c r="Q15" s="34"/>
-      <c r="R15" s="34"/>
+      <c r="R15" s="34">
+        <v>1</v>
+      </c>
       <c r="S15" s="35"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1">
@@ -35900,9 +35922,12 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="54" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="18" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -35913,19 +35938,20 @@
   </sheetPr>
   <dimension ref="A1:S988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView view="pageBreakPreview" topLeftCell="B1" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="7.77734375" customWidth="1"/>
-    <col min="3" max="3" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="52.5546875" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.21875" customWidth="1"/>
     <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="9" width="10.21875" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="11" max="11" width="10.77734375" customWidth="1"/>
     <col min="12" max="13" width="10.21875" customWidth="1"/>
@@ -36296,14 +36322,22 @@
       <c r="D13" s="96">
         <v>4</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="34">
+        <v>1</v>
+      </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="34">
+        <v>1</v>
+      </c>
       <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="J13" s="34">
+        <v>1</v>
+      </c>
       <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
+      <c r="L13" s="34">
+        <v>1</v>
+      </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
@@ -36329,7 +36363,9 @@
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="I14" s="34">
+        <v>1</v>
+      </c>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
@@ -36358,7 +36394,9 @@
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="I15" s="34">
+        <v>2</v>
+      </c>
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="34"/>
@@ -36389,7 +36427,9 @@
       <c r="H16" s="34"/>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
+      <c r="K16" s="34">
+        <v>2</v>
+      </c>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
       <c r="N16" s="34"/>
@@ -36448,43 +36488,43 @@
       </c>
       <c r="I18" s="44">
         <f>IF(COUNTA(I14:I16)&gt;0,SUM(I14:I16),G18)</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="J18" s="44">
         <f t="shared" ref="J18:L18" si="5">IF(COUNTA(J14:J16)&gt;0,SUM(J14:J16),I18)</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="K18" s="44">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="L18" s="44">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M18" s="44">
         <f>IF(COUNTA(M14:M16)&gt;0,SUM(M14:M16),K18)</f>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N18" s="44">
         <f t="shared" ref="N18:O18" si="6">IF(COUNTA(N14:N16)&gt;0,SUM(N14:N16),M18)</f>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="O18" s="44">
         <f t="shared" si="6"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="P18" s="44">
         <f t="shared" ref="P18:R18" si="7">IF(COUNTA(P14:P16)&gt;0,SUM(P14:P16),N18)</f>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="44">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="R18" s="44">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="S18" s="28"/>
     </row>
@@ -36578,7 +36618,7 @@
       </c>
       <c r="I20" s="34">
         <f>G18-I18</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="J20" s="34">
         <f t="shared" ref="J20:L20" si="10">I18-J18</f>
@@ -36586,7 +36626,7 @@
       </c>
       <c r="K20" s="34">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="34">
         <f t="shared" si="10"/>
@@ -37713,9 +37753,12 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="55" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="18" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -37726,7 +37769,9 @@
   </sheetPr>
   <dimension ref="A1:S987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -39495,9 +39540,12 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="18" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -39508,7 +39556,7 @@
   </sheetPr>
   <dimension ref="A1:S988"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -41298,9 +41346,12 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup scale="59" orientation="landscape" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="18" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>